<commit_message>
added three candidates' contact info.
</commit_message>
<xml_diff>
--- a/2019坊新招聘候选人列表_ver1.0.xlsx
+++ b/2019坊新招聘候选人列表_ver1.0.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414AF763-EC88-4845-8694-F9BD4CE9EACC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 Q1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="70">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -240,23 +241,57 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>陈蒙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhongliansanguo@foxmail.com</t>
+  </si>
+  <si>
+    <t>中专</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>582641020@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本科</t>
+  </si>
+  <si>
+    <t>黄洪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1264339765@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>室内设计, 国家注册高级设计师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -272,7 +307,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,7 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -369,10 +404,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -649,32 +687,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="52.28515625" customWidth="1"/>
-    <col min="11" max="15" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="7.75" customWidth="1"/>
+    <col min="7" max="7" width="5.375" customWidth="1"/>
+    <col min="8" max="8" width="11.25" customWidth="1"/>
+    <col min="9" max="9" width="28.5" customWidth="1"/>
+    <col min="10" max="10" width="52.25" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="8.125" customWidth="1"/>
+    <col min="13" max="13" width="8.625" customWidth="1"/>
+    <col min="14" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
     <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="19" max="19" width="9.875" customWidth="1"/>
     <col min="20" max="20" width="31" customWidth="1"/>
-    <col min="21" max="21" width="121.140625" customWidth="1"/>
+    <col min="21" max="21" width="121.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5">
+    <row r="1" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -739,7 +782,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="33">
+    <row r="2" spans="1:21" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
@@ -798,7 +841,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="66">
+    <row r="3" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -855,7 +898,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="66">
+    <row r="4" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
@@ -912,7 +955,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="66">
+    <row r="5" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -969,7 +1012,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="66">
+    <row r="6" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -1028,7 +1071,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="66">
+    <row r="7" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>27</v>
       </c>
@@ -1087,7 +1130,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="66">
+    <row r="8" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1143,17 +1186,178 @@
       <c r="U8" s="10" t="s">
         <v>47</v>
       </c>
+    </row>
+    <row r="9" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="12">
+        <v>43578</v>
+      </c>
+      <c r="E9" s="1">
+        <v>18701914478</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="1">
+        <v>30</v>
+      </c>
+      <c r="H9" s="4">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R9" s="1"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+    </row>
+    <row r="10" spans="1:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="12">
+        <v>43578</v>
+      </c>
+      <c r="E10" s="1">
+        <v>17316360798</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="1">
+        <v>26</v>
+      </c>
+      <c r="H10" s="4">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+    </row>
+    <row r="11" spans="1:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="12">
+        <v>43578</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>33</v>
+      </c>
+      <c r="H11" s="4">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" s="5"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J6" r:id="rId2"/>
-    <hyperlink ref="J7" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="B3:B8" r:id="rId5" display="hubinglei@jijiangspace.com"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B3:B8" r:id="rId5" display="hubinglei@jijiangspace.com" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{5AD9CC02-426E-4FE3-91C0-0B414356C275}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{CA9E727B-E4F6-49C8-A8D0-B3EE072A9992}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>